<commit_message>
new results - pattern based
</commit_message>
<xml_diff>
--- a/experiments/Pattern-BasedRepair.xlsx
+++ b/experiments/Pattern-BasedRepair.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgopinat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musman\Desktop\DNN-Repair\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD4C07-765B-45EC-B16F-78EEDE9411DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF26EFDB-643D-480F-9CDB-434A514DAB6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E851A2A-318E-4F15-AEB0-BD2CB026064A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6E851A2A-318E-4F15-AEB0-BD2CB026064A}"/>
   </bookViews>
   <sheets>
     <sheet name="PatternBasedRepair" sheetId="1" r:id="rId1"/>
     <sheet name="wTestSet" sheetId="10" r:id="rId2"/>
+    <sheet name="Summary" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>LABEL 7</t>
   </si>
@@ -150,47 +151,62 @@
     <t>95.5454698268616,94.94549058473737</t>
   </si>
   <si>
-    <t>99.0258075542642,98.66529774127311</t>
-  </si>
-  <si>
-    <t>99.9840383080606,98.73540856031128</t>
-  </si>
-  <si>
-    <t>99.0368367691787,98.64300626304802</t>
-  </si>
-  <si>
-    <t>98.985427042981,98.65470852017937</t>
-  </si>
-  <si>
-    <t>98.8702499144128,98.77800407331976</t>
-  </si>
-  <si>
-    <t>98.9561246126243,98.8118811881188</t>
-  </si>
-  <si>
-    <t>98.7747566297415,97.86821705426357</t>
-  </si>
-  <si>
-    <t>98.7095817264906,99.47136563876651</t>
-  </si>
-  <si>
-    <t>98.9701164950194,99.38775510204081</t>
-  </si>
-  <si>
-    <t>98.9883333333333,98.63</t>
-  </si>
-  <si>
     <t>96.5783333333333,96.34</t>
   </si>
   <si>
-    <t>98.55437888720793,97.22497522299307</t>
+    <t>POISONED-TESTSET (Original)</t>
+  </si>
+  <si>
+    <t>POISONED-TESTSET (Poisoned)</t>
+  </si>
+  <si>
+    <t>Label 0</t>
+  </si>
+  <si>
+    <t>Label 1</t>
+  </si>
+  <si>
+    <t>Label 2</t>
+  </si>
+  <si>
+    <t>Label 3</t>
+  </si>
+  <si>
+    <t>Label 4</t>
+  </si>
+  <si>
+    <t>Label 5</t>
+  </si>
+  <si>
+    <t>Label 6</t>
+  </si>
+  <si>
+    <t>Label 7</t>
+  </si>
+  <si>
+    <t>Label 8</t>
+  </si>
+  <si>
+    <t>Label 9</t>
+  </si>
+  <si>
+    <t>Poisoned</t>
+  </si>
+  <si>
+    <t>TrainSet</t>
+  </si>
+  <si>
+    <t>TestSet</t>
+  </si>
+  <si>
+    <t>TestSet - Poisoned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +231,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -222,15 +239,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,15 +284,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6208AF9-2615-483A-B970-BCAA536C0A4F}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,38 +1133,38 @@
       <c r="A16">
         <v>0</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="7">
         <v>98.970116495019397</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="12">
         <v>98.9869998311666</v>
       </c>
-      <c r="D16" s="5">
-        <v>98.919466486577704</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="D16" s="9">
+        <v>98.868816478135997</v>
+      </c>
+      <c r="E16" s="9">
         <v>98.936349822724907</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="9">
         <v>97.568799594799899</v>
       </c>
-      <c r="G16">
-        <v>97.70386628</v>
-      </c>
-      <c r="H16">
-        <v>96.488266080000002</v>
-      </c>
-      <c r="I16">
-        <v>98.311666389999999</v>
-      </c>
-      <c r="J16">
+      <c r="G16" s="9">
+        <v>97.703866283977703</v>
+      </c>
+      <c r="H16" s="9">
+        <v>98.159716359952697</v>
+      </c>
+      <c r="I16" s="9">
+        <v>98.294783049130501</v>
+      </c>
+      <c r="J16" s="9">
         <v>98.970116495019397</v>
       </c>
-      <c r="K16">
-        <v>97.872699645449899</v>
-      </c>
-      <c r="L16">
-        <v>98.953233158872195</v>
+      <c r="K16" s="9">
+        <v>97.788282964713801</v>
+      </c>
+      <c r="L16" s="8">
+        <v>99.003883167313802</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1135,38 +1172,38 @@
         <f>A16+1</f>
         <v>1</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="7">
         <v>98.709581726490597</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="8">
         <v>98.739246514387403</v>
       </c>
-      <c r="D17" s="1">
-        <v>98.798576090180902</v>
-      </c>
-      <c r="E17">
+      <c r="D17" s="12">
+        <v>98.872738059922796</v>
+      </c>
+      <c r="E17" s="9">
         <v>98.531592999110003</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="9">
         <v>98.398101453574597</v>
       </c>
-      <c r="G17">
-        <v>98.605754970000007</v>
-      </c>
-      <c r="H17">
-        <v>98.783743700000002</v>
-      </c>
-      <c r="I17">
-        <v>98.353604270000005</v>
-      </c>
-      <c r="J17">
+      <c r="G17" s="9">
+        <v>98.605754968851898</v>
+      </c>
+      <c r="H17" s="8">
+        <v>98.739246514387403</v>
+      </c>
+      <c r="I17" s="7">
+        <v>98.427766241471303</v>
+      </c>
+      <c r="J17" s="9">
         <v>98.709581726490597</v>
       </c>
-      <c r="K17">
-        <v>98.709581726490597</v>
-      </c>
-      <c r="L17">
-        <v>98.754078908335799</v>
+      <c r="K17" s="8">
+        <v>98.739246514387403</v>
+      </c>
+      <c r="L17" s="8">
+        <v>98.768911302284195</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1174,38 +1211,38 @@
         <f t="shared" ref="A18:A25" si="1">A17+1</f>
         <v>2</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="7">
         <v>98.774756629741503</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>98.657267539442699</v>
       </c>
-      <c r="D18">
-        <v>98.657267539442699</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D18" s="9">
+        <v>98.606915072171802</v>
+      </c>
+      <c r="E18" s="12">
         <v>98.858677408526304</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="9">
         <v>89.610607586438405</v>
       </c>
-      <c r="G18">
-        <v>98.774756629999999</v>
-      </c>
-      <c r="H18">
-        <v>92.967438740000006</v>
-      </c>
-      <c r="I18">
-        <v>98.657267540000007</v>
-      </c>
-      <c r="J18">
+      <c r="G18" s="9">
         <v>98.774756629741503</v>
       </c>
-      <c r="K18">
+      <c r="H18" s="9">
+        <v>94.528365223229201</v>
+      </c>
+      <c r="I18" s="9">
         <v>98.539778449143995</v>
       </c>
-      <c r="L18">
+      <c r="J18" s="9">
         <v>98.774756629741503</v>
+      </c>
+      <c r="K18" s="9">
+        <v>98.506210137630006</v>
+      </c>
+      <c r="L18" s="9">
+        <v>98.741188318227501</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1213,38 +1250,38 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="7">
         <v>98.956124612624293</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>98.874571847985607</v>
       </c>
-      <c r="D19">
-        <v>98.923503506768796</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="9">
+        <v>98.939814059696602</v>
+      </c>
+      <c r="E19" s="9">
         <v>98.874571847985607</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="12">
         <v>99.217093459468202</v>
       </c>
-      <c r="G19">
-        <v>98.71146632</v>
-      </c>
-      <c r="H19">
-        <v>97.227205999999995</v>
-      </c>
-      <c r="I19">
-        <v>98.678845210000006</v>
-      </c>
-      <c r="J19">
+      <c r="G19" s="9">
+        <v>98.711466318708204</v>
+      </c>
+      <c r="H19" s="9">
+        <v>98.059044201598397</v>
+      </c>
+      <c r="I19" s="9">
+        <v>98.662534659924901</v>
+      </c>
+      <c r="J19" s="9">
         <v>98.939814059696602</v>
       </c>
-      <c r="K19">
-        <v>98.907192953841104</v>
-      </c>
-      <c r="L19">
-        <v>98.988745718479805</v>
+      <c r="K19" s="8">
+        <v>98.972435165552099</v>
+      </c>
+      <c r="L19" s="8">
+        <v>98.972435165552099</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1252,38 +1289,38 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="7">
         <v>98.870249914412796</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>98.699075659020806</v>
       </c>
-      <c r="D20">
-        <v>98.784662786716794</v>
-      </c>
-      <c r="E20">
+      <c r="D20" s="9">
+        <v>98.733310510099201</v>
+      </c>
+      <c r="E20" s="9">
         <v>98.801780212256006</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="9">
         <v>98.818897637795203</v>
       </c>
-      <c r="G20" s="1">
-        <v>98.921602190000002</v>
-      </c>
-      <c r="H20">
-        <v>97.107155079999998</v>
-      </c>
-      <c r="I20">
-        <v>98.476549129999995</v>
-      </c>
-      <c r="J20">
+      <c r="G20" s="12">
+        <v>98.921602191030402</v>
+      </c>
+      <c r="H20" s="9">
+        <v>98.288257446080095</v>
+      </c>
+      <c r="I20" s="9">
+        <v>98.476549127011296</v>
+      </c>
+      <c r="J20" s="9">
         <v>98.836015063334401</v>
       </c>
-      <c r="K20">
-        <v>98.271140020540898</v>
-      </c>
-      <c r="L20">
-        <v>97.637795275590506</v>
+      <c r="K20" s="9">
+        <v>98.459431701472099</v>
+      </c>
+      <c r="L20" s="9">
+        <v>98.442314275932901</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1291,38 +1328,38 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="7">
         <v>98.985427042981001</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>98.468917173953102</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="9">
+        <v>98.9485334809075</v>
+      </c>
+      <c r="E21" s="9">
+        <v>98.985427042981001</v>
+      </c>
+      <c r="F21" s="9">
+        <v>97.509684560044207</v>
+      </c>
+      <c r="G21" s="9">
+        <v>98.985427042981001</v>
+      </c>
+      <c r="H21" s="13">
         <v>98.966980261944201</v>
       </c>
-      <c r="E21">
+      <c r="I21" s="9">
         <v>98.985427042981001</v>
       </c>
-      <c r="F21">
-        <v>97.509684560044207</v>
-      </c>
-      <c r="G21">
-        <v>98.985427040000005</v>
-      </c>
-      <c r="H21" s="1">
-        <v>99.151448070000001</v>
-      </c>
-      <c r="I21">
-        <v>98.911639919999999</v>
-      </c>
-      <c r="J21">
+      <c r="J21" s="9">
         <v>98.966980261944201</v>
       </c>
-      <c r="K21">
-        <v>96.919387566869503</v>
-      </c>
-      <c r="L21">
-        <v>97.6572588083379</v>
+      <c r="K21" s="9">
+        <v>96.900940785832802</v>
+      </c>
+      <c r="L21" s="9">
+        <v>98.284449363586006</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1330,38 +1367,38 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="7">
         <v>99.036836769178706</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="8">
         <v>99.053734369719507</v>
       </c>
-      <c r="D22" s="5">
-        <v>99.053734369719507</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="9">
+        <v>99.036836769178706</v>
+      </c>
+      <c r="E22" s="9">
         <v>99.019939168638004</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="9">
         <v>98.698884758364301</v>
       </c>
-      <c r="G22">
-        <v>99.036836769999994</v>
-      </c>
-      <c r="H22">
-        <v>93.105778979999997</v>
-      </c>
-      <c r="I22" s="7">
-        <v>99.003041569999993</v>
-      </c>
-      <c r="J22">
+      <c r="G22" s="9">
         <v>99.036836769178706</v>
       </c>
-      <c r="K22">
-        <v>98.732679959445704</v>
-      </c>
-      <c r="L22">
-        <v>98.614396755660593</v>
+      <c r="H22" s="9">
+        <v>95.2010814464346</v>
+      </c>
+      <c r="I22" s="12">
+        <v>99.070631970260195</v>
+      </c>
+      <c r="J22" s="9">
+        <v>99.036836769178706</v>
+      </c>
+      <c r="K22" s="9">
+        <v>98.766475160527193</v>
+      </c>
+      <c r="L22" s="9">
+        <v>98.8340655626901</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1369,38 +1406,38 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="7">
         <v>99.984038308060605</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>99.728651237031102</v>
       </c>
-      <c r="D23">
-        <v>99.169992019153995</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="7">
+        <v>98.595371109337506</v>
+      </c>
+      <c r="E23" s="9">
         <v>99.824421388667105</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="9">
         <v>98.786911412609697</v>
       </c>
-      <c r="G23">
-        <v>98.324022350000007</v>
-      </c>
-      <c r="H23">
-        <v>98.627294489999997</v>
-      </c>
-      <c r="I23">
-        <v>99.872306460000004</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="G23" s="9">
+        <v>98.292098962490002</v>
+      </c>
+      <c r="H23" s="9">
+        <v>99.680766161213</v>
+      </c>
+      <c r="I23" s="9">
+        <v>99.824421388667105</v>
+      </c>
+      <c r="J23" s="12">
         <v>100</v>
       </c>
-      <c r="K23">
-        <v>99.600957701516293</v>
-      </c>
-      <c r="L23">
-        <v>97.621707901037496</v>
+      <c r="K23" s="9">
+        <v>99.553072625698306</v>
+      </c>
+      <c r="L23" s="9">
+        <v>99.0422984836392</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -1408,38 +1445,38 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="7">
         <v>99.025807554264205</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="9">
         <v>98.991625363185705</v>
       </c>
-      <c r="D24" s="5">
-        <v>98.991625363185705</v>
-      </c>
-      <c r="E24">
+      <c r="D24" s="9">
+        <v>98.906169885489604</v>
+      </c>
+      <c r="E24" s="9">
         <v>99.008716458725004</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="9">
         <v>98.427619210391299</v>
       </c>
-      <c r="G24">
-        <v>97.62433772</v>
-      </c>
-      <c r="H24">
-        <v>56.058793369999997</v>
-      </c>
-      <c r="I24">
-        <v>98.581439070000002</v>
-      </c>
-      <c r="J24">
+      <c r="G24" s="9">
+        <v>97.624337720047805</v>
+      </c>
+      <c r="H24" s="9">
+        <v>81.063066142539697</v>
+      </c>
+      <c r="I24" s="9">
+        <v>97.555973337890904</v>
+      </c>
+      <c r="J24" s="9">
         <v>98.632712356862001</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="12">
         <v>99.111263031960306</v>
       </c>
-      <c r="L24">
-        <v>98.752350025636602</v>
+      <c r="L24" s="9">
+        <v>98.632712356862001</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -1447,46 +1484,43 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="7">
         <v>98.554378887207903</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
         <v>98.369473861153097</v>
       </c>
-      <c r="D25">
-        <v>97.629853756933898</v>
-      </c>
-      <c r="E25">
+      <c r="D25" s="9">
+        <v>97.579425113464396</v>
+      </c>
+      <c r="E25" s="9">
         <v>98.352664313329896</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="9">
         <v>97.663472852580199</v>
       </c>
-      <c r="G25">
-        <v>97.528996469999996</v>
-      </c>
-      <c r="H25">
-        <v>96.385947220000006</v>
-      </c>
-      <c r="I25">
-        <v>98.050092449999994</v>
-      </c>
-      <c r="J25">
+      <c r="G25" s="9">
+        <v>97.528996469994894</v>
+      </c>
+      <c r="H25" s="9">
+        <v>98.167759287275103</v>
+      </c>
+      <c r="I25" s="9">
+        <v>98.050092452512999</v>
+      </c>
+      <c r="J25" s="9">
         <v>97.226424609177997</v>
       </c>
-      <c r="K25">
-        <v>96.957471844007301</v>
-      </c>
-      <c r="L25" s="7">
-        <v>96.100184905025998</v>
+      <c r="K25" s="9">
+        <v>96.923852748361</v>
+      </c>
+      <c r="L25" s="13">
+        <v>96.755757270129394</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B26">
-        <v>98.988333333333301</v>
       </c>
     </row>
   </sheetData>
@@ -1497,20 +1531,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6816E6FB-2578-42FA-A216-5F0E87175422}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L26"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -1546,7 +1584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1584,7 +1622,7 @@
         <v>98.548033091338795</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>A3+1</f>
         <v>1</v>
@@ -1623,7 +1661,7 @@
         <v>97.626816968258595</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" ref="A5:A12" si="0">A4+1</f>
         <v>2</v>
@@ -1662,7 +1700,7 @@
         <v>97.197045988586694</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1701,7 +1739,7 @@
         <v>95.302560756809598</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1740,7 +1778,7 @@
         <v>98.339609722697702</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1779,7 +1817,7 @@
         <v>98.395130049806298</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1818,7 +1856,7 @@
         <v>97.194998310239896</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1857,7 +1895,7 @@
         <v>94.014365522745393</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1896,7 +1934,7 @@
         <v>91.556998803623301</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1935,12 +1973,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C13">
         <v>96.481666666666598</v>
@@ -1955,13 +1993,13 @@
         <v>90.86</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>6</v>
@@ -1979,16 +2017,16 @@
         <v>11</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>13</v>
@@ -1996,43 +2034,51 @@
       <c r="L15" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1">
-        <v>98.9869998311666</v>
-      </c>
-      <c r="D16" s="5">
-        <v>98.919466486577704</v>
-      </c>
-      <c r="E16" s="5">
-        <v>98.936349822724907</v>
-      </c>
-      <c r="F16" s="5">
-        <v>97.568799594799899</v>
-      </c>
-      <c r="G16">
-        <v>97.70386628</v>
-      </c>
-      <c r="H16">
-        <v>96.488266080000002</v>
-      </c>
-      <c r="I16">
-        <v>98.311666389999999</v>
-      </c>
-      <c r="J16">
-        <v>98.970116495019397</v>
-      </c>
-      <c r="K16">
-        <v>97.872699645449899</v>
-      </c>
-      <c r="L16">
-        <v>98.953233158872195</v>
+      <c r="B16" s="7">
+        <v>99.387755102040799</v>
+      </c>
+      <c r="C16" s="12">
+        <v>99.5918367346938</v>
+      </c>
+      <c r="D16" s="9">
+        <v>99.183673469387699</v>
+      </c>
+      <c r="E16" s="9">
+        <v>99.285714285714207</v>
+      </c>
+      <c r="F16" s="9">
+        <v>97.448979591836704</v>
+      </c>
+      <c r="G16" s="9">
+        <v>98.367346938775498</v>
+      </c>
+      <c r="H16" s="9">
+        <v>98.571428571428498</v>
+      </c>
+      <c r="I16" s="9">
+        <v>98.673469387755006</v>
+      </c>
+      <c r="J16" s="9">
+        <v>99.387755102040799</v>
+      </c>
+      <c r="K16" s="9">
+        <v>98.673469387755006</v>
+      </c>
+      <c r="L16" s="8">
+        <v>99.5918367346938</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2040,38 +2086,38 @@
         <f>A16+1</f>
         <v>1</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17">
-        <v>98.739246514387403</v>
-      </c>
-      <c r="D17" s="1">
-        <v>98.798576090180902</v>
-      </c>
-      <c r="E17">
-        <v>98.531592999110003</v>
-      </c>
-      <c r="F17">
-        <v>98.398101453574597</v>
-      </c>
-      <c r="G17">
-        <v>98.605754970000007</v>
-      </c>
-      <c r="H17">
-        <v>98.783743700000002</v>
-      </c>
-      <c r="I17">
-        <v>98.353604270000005</v>
-      </c>
-      <c r="J17">
-        <v>98.709581726490597</v>
-      </c>
-      <c r="K17">
-        <v>98.709581726490597</v>
-      </c>
-      <c r="L17">
-        <v>98.754078908335799</v>
+      <c r="B17" s="7">
+        <v>99.4713656387665</v>
+      </c>
+      <c r="C17" s="9">
+        <v>99.2070484581497</v>
+      </c>
+      <c r="D17" s="12">
+        <v>99.647577092511</v>
+      </c>
+      <c r="E17" s="9">
+        <v>98.766519823788499</v>
+      </c>
+      <c r="F17" s="9">
+        <v>99.2070484581497</v>
+      </c>
+      <c r="G17" s="9">
+        <v>99.3832599118942</v>
+      </c>
+      <c r="H17" s="8">
+        <v>99.647577092511</v>
+      </c>
+      <c r="I17" s="9">
+        <v>98.678414096916299</v>
+      </c>
+      <c r="J17" s="9">
+        <v>99.4713656387665</v>
+      </c>
+      <c r="K17" s="9">
+        <v>98.678414096916299</v>
+      </c>
+      <c r="L17" s="8">
+        <v>99.647577092511</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2079,38 +2125,38 @@
         <f t="shared" ref="A18:A25" si="1">A17+1</f>
         <v>2</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18">
-        <v>98.657267539442699</v>
-      </c>
-      <c r="D18">
-        <v>98.657267539442699</v>
-      </c>
-      <c r="E18" s="1">
-        <v>98.858677408526304</v>
-      </c>
-      <c r="F18">
-        <v>89.610607586438405</v>
-      </c>
-      <c r="G18">
-        <v>98.774756629999999</v>
-      </c>
-      <c r="H18">
-        <v>92.967438740000006</v>
-      </c>
-      <c r="I18">
-        <v>98.657267540000007</v>
-      </c>
-      <c r="J18">
-        <v>98.774756629741503</v>
-      </c>
-      <c r="K18">
-        <v>98.539778449143995</v>
-      </c>
-      <c r="L18">
-        <v>98.774756629741503</v>
+      <c r="B18" s="7">
+        <v>97.868217054263496</v>
+      </c>
+      <c r="C18" s="9">
+        <v>97.480620155038693</v>
+      </c>
+      <c r="D18" s="9">
+        <v>97.771317829457303</v>
+      </c>
+      <c r="E18" s="12">
+        <v>98.546511627906895</v>
+      </c>
+      <c r="F18" s="9">
+        <v>86.143410852713103</v>
+      </c>
+      <c r="G18" s="8">
+        <v>98.643410852713103</v>
+      </c>
+      <c r="H18" s="9">
+        <v>92.054263565891404</v>
+      </c>
+      <c r="I18" s="8">
+        <v>98.158914728682106</v>
+      </c>
+      <c r="J18" s="8">
+        <v>97.965116279069704</v>
+      </c>
+      <c r="K18" s="9">
+        <v>97.383720930232499</v>
+      </c>
+      <c r="L18" s="8">
+        <v>97.965116279069704</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2118,38 +2164,38 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19">
-        <v>98.874571847985607</v>
-      </c>
-      <c r="D19">
-        <v>98.923503506768796</v>
-      </c>
-      <c r="E19">
-        <v>98.874571847985607</v>
-      </c>
-      <c r="F19" s="1">
-        <v>99.217093459468202</v>
-      </c>
-      <c r="G19">
-        <v>98.71146632</v>
-      </c>
-      <c r="H19">
-        <v>97.227205999999995</v>
-      </c>
-      <c r="I19">
-        <v>98.678845210000006</v>
-      </c>
-      <c r="J19">
-        <v>98.939814059696602</v>
-      </c>
-      <c r="K19">
-        <v>98.907192953841104</v>
-      </c>
-      <c r="L19">
-        <v>98.988745718479805</v>
+      <c r="B19" s="7">
+        <v>98.811881188118804</v>
+      </c>
+      <c r="C19" s="9">
+        <v>98.811881188118804</v>
+      </c>
+      <c r="D19" s="9">
+        <v>98.613861386138595</v>
+      </c>
+      <c r="E19" s="8">
+        <v>99.009900990098998</v>
+      </c>
+      <c r="F19" s="12">
+        <v>99.405940594059402</v>
+      </c>
+      <c r="G19" s="9">
+        <v>98.4158415841584</v>
+      </c>
+      <c r="H19" s="9">
+        <v>97.524752475247496</v>
+      </c>
+      <c r="I19" s="9">
+        <v>98.514851485148498</v>
+      </c>
+      <c r="J19" s="8">
+        <v>98.910891089108901</v>
+      </c>
+      <c r="K19" s="9">
+        <v>98.712871287128706</v>
+      </c>
+      <c r="L19" s="8">
+        <v>99.306930693069305</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2157,38 +2203,38 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20">
-        <v>98.699075659020806</v>
-      </c>
-      <c r="D20">
-        <v>98.784662786716794</v>
-      </c>
-      <c r="E20">
-        <v>98.801780212256006</v>
-      </c>
-      <c r="F20">
-        <v>98.818897637795203</v>
-      </c>
-      <c r="G20" s="1">
-        <v>98.921602190000002</v>
-      </c>
-      <c r="H20">
-        <v>97.107155079999998</v>
-      </c>
-      <c r="I20">
-        <v>98.476549129999995</v>
-      </c>
-      <c r="J20">
-        <v>98.836015063334401</v>
-      </c>
-      <c r="K20">
-        <v>98.271140020540898</v>
-      </c>
-      <c r="L20">
-        <v>97.637795275590506</v>
+      <c r="B20" s="7">
+        <v>98.778004073319707</v>
+      </c>
+      <c r="C20" s="8">
+        <v>98.981670061099706</v>
+      </c>
+      <c r="D20" s="8">
+        <v>98.879837067209706</v>
+      </c>
+      <c r="E20" s="9">
+        <v>98.778004073319707</v>
+      </c>
+      <c r="F20" s="8">
+        <v>98.981670061099706</v>
+      </c>
+      <c r="G20" s="12">
+        <v>99.694501018329902</v>
+      </c>
+      <c r="H20" s="9">
+        <v>98.370672097759595</v>
+      </c>
+      <c r="I20" s="9">
+        <v>98.676171079429693</v>
+      </c>
+      <c r="J20" s="9">
+        <v>98.778004073319707</v>
+      </c>
+      <c r="K20" s="9">
+        <v>98.676171079429693</v>
+      </c>
+      <c r="L20" s="9">
+        <v>98.574338085539694</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2196,38 +2242,38 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
-        <v>98.468917173953102</v>
-      </c>
-      <c r="D21">
-        <v>98.966980261944201</v>
-      </c>
-      <c r="E21">
-        <v>98.985427042981001</v>
-      </c>
-      <c r="F21">
-        <v>97.509684560044207</v>
-      </c>
-      <c r="G21">
-        <v>98.985427040000005</v>
-      </c>
-      <c r="H21" s="1">
-        <v>99.151448070000001</v>
-      </c>
-      <c r="I21">
-        <v>98.911639919999999</v>
-      </c>
-      <c r="J21">
-        <v>98.966980261944201</v>
-      </c>
-      <c r="K21">
-        <v>96.919387566869503</v>
-      </c>
-      <c r="L21">
-        <v>97.6572588083379</v>
+      <c r="B21" s="7">
+        <v>98.654708520179298</v>
+      </c>
+      <c r="C21" s="9">
+        <v>97.645739910313907</v>
+      </c>
+      <c r="D21" s="9">
+        <v>98.430493273542595</v>
+      </c>
+      <c r="E21" s="9">
+        <v>98.542600896860904</v>
+      </c>
+      <c r="F21" s="9">
+        <v>96.300448430493205</v>
+      </c>
+      <c r="G21" s="9">
+        <v>98.654708520179298</v>
+      </c>
+      <c r="H21" s="12">
+        <v>99.327354260089606</v>
+      </c>
+      <c r="I21" s="9">
+        <v>98.654708520179298</v>
+      </c>
+      <c r="J21" s="9">
+        <v>98.654708520179298</v>
+      </c>
+      <c r="K21" s="9">
+        <v>96.188340807174797</v>
+      </c>
+      <c r="L21" s="9">
+        <v>97.645739910313907</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2235,38 +2281,38 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="1">
-        <v>99.053734369719507</v>
-      </c>
-      <c r="D22" s="5">
-        <v>99.053734369719507</v>
-      </c>
-      <c r="E22">
-        <v>99.019939168638004</v>
-      </c>
-      <c r="F22">
-        <v>98.698884758364301</v>
-      </c>
-      <c r="G22">
-        <v>99.036836769999994</v>
-      </c>
-      <c r="H22">
-        <v>93.105778979999997</v>
-      </c>
-      <c r="I22" s="7">
-        <v>99.003041569999993</v>
-      </c>
-      <c r="J22">
-        <v>99.036836769178706</v>
-      </c>
-      <c r="K22">
-        <v>98.732679959445704</v>
-      </c>
-      <c r="L22">
-        <v>98.614396755660593</v>
+      <c r="B22" s="7">
+        <v>98.643006263047994</v>
+      </c>
+      <c r="C22" s="8">
+        <v>99.060542797494705</v>
+      </c>
+      <c r="D22" s="9">
+        <v>98.434237995824603</v>
+      </c>
+      <c r="E22" s="8">
+        <v>98.956158663883002</v>
+      </c>
+      <c r="F22" s="9">
+        <v>97.807933194154401</v>
+      </c>
+      <c r="G22" s="8">
+        <v>98.747390396659696</v>
+      </c>
+      <c r="H22" s="9">
+        <v>93.736951983298496</v>
+      </c>
+      <c r="I22" s="12">
+        <v>99.373695198329798</v>
+      </c>
+      <c r="J22" s="9">
+        <v>98.643006263047994</v>
+      </c>
+      <c r="K22" s="9">
+        <v>98.538622129436305</v>
+      </c>
+      <c r="L22" s="9">
+        <v>98.3298538622129</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2274,38 +2320,38 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23">
-        <v>99.728651237031102</v>
-      </c>
-      <c r="D23">
-        <v>99.169992019153995</v>
-      </c>
-      <c r="E23">
-        <v>99.824421388667105</v>
-      </c>
-      <c r="F23">
-        <v>98.786911412609697</v>
-      </c>
-      <c r="G23">
-        <v>98.324022350000007</v>
-      </c>
-      <c r="H23">
-        <v>98.627294489999997</v>
-      </c>
-      <c r="I23">
-        <v>99.872306460000004</v>
-      </c>
-      <c r="J23" s="1">
-        <v>100</v>
-      </c>
-      <c r="K23">
-        <v>99.600957701516293</v>
-      </c>
-      <c r="L23">
-        <v>97.621707901037496</v>
+      <c r="B23" s="7">
+        <v>98.7354085603112</v>
+      </c>
+      <c r="C23" s="9">
+        <v>98.054474708171199</v>
+      </c>
+      <c r="D23" s="9">
+        <v>97.081712062256798</v>
+      </c>
+      <c r="E23" s="9">
+        <v>98.346303501945499</v>
+      </c>
+      <c r="F23" s="9">
+        <v>97.568093385213999</v>
+      </c>
+      <c r="G23" s="9">
+        <v>96.984435797665299</v>
+      </c>
+      <c r="H23" s="9">
+        <v>97.762645914396799</v>
+      </c>
+      <c r="I23" s="9">
+        <v>98.443579766536899</v>
+      </c>
+      <c r="J23" s="13">
+        <v>98.7354085603112</v>
+      </c>
+      <c r="K23" s="9">
+        <v>97.762645914396799</v>
+      </c>
+      <c r="L23" s="9">
+        <v>97.276264591439599</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2313,38 +2359,38 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="5">
-        <v>98.991625363185705</v>
-      </c>
-      <c r="D24" s="5">
-        <v>98.991625363185705</v>
-      </c>
-      <c r="E24">
-        <v>99.008716458725004</v>
-      </c>
-      <c r="F24">
-        <v>98.427619210391299</v>
-      </c>
-      <c r="G24">
-        <v>97.62433772</v>
-      </c>
-      <c r="H24">
-        <v>56.058793369999997</v>
-      </c>
-      <c r="I24">
-        <v>98.581439070000002</v>
-      </c>
-      <c r="J24">
-        <v>98.632712356862001</v>
-      </c>
-      <c r="K24" s="1">
-        <v>99.111263031960306</v>
-      </c>
-      <c r="L24">
-        <v>98.752350025636602</v>
+      <c r="B24" s="7">
+        <v>98.665297741273093</v>
+      </c>
+      <c r="C24" s="9">
+        <v>98.459958932238195</v>
+      </c>
+      <c r="D24" s="9">
+        <v>98.562628336755594</v>
+      </c>
+      <c r="E24" s="9">
+        <v>98.254620123203196</v>
+      </c>
+      <c r="F24" s="9">
+        <v>97.5359342915811</v>
+      </c>
+      <c r="G24" s="9">
+        <v>97.433264887063601</v>
+      </c>
+      <c r="H24" s="9">
+        <v>81.930184804928103</v>
+      </c>
+      <c r="I24" s="9">
+        <v>96.611909650924005</v>
+      </c>
+      <c r="J24" s="9">
+        <v>98.254620123203196</v>
+      </c>
+      <c r="K24" s="12">
+        <v>99.178644763860305</v>
+      </c>
+      <c r="L24" s="9">
+        <v>97.741273100615999</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2352,49 +2398,649 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25">
-        <v>98.369473861153097</v>
-      </c>
-      <c r="D25">
-        <v>97.629853756933898</v>
-      </c>
-      <c r="E25">
-        <v>98.352664313329896</v>
-      </c>
-      <c r="F25">
-        <v>97.663472852580199</v>
-      </c>
-      <c r="G25">
-        <v>97.528996469999996</v>
-      </c>
-      <c r="H25">
-        <v>96.385947220000006</v>
-      </c>
-      <c r="I25">
-        <v>98.050092449999994</v>
-      </c>
-      <c r="J25">
-        <v>97.226424609177997</v>
-      </c>
-      <c r="K25">
-        <v>96.957471844007301</v>
-      </c>
-      <c r="L25" s="7">
-        <v>96.100184905025998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="7">
+        <v>97.224975222992995</v>
+      </c>
+      <c r="C25" s="9">
+        <v>96.630327056491495</v>
+      </c>
+      <c r="D25" s="9">
+        <v>96.630327056491495</v>
+      </c>
+      <c r="E25" s="9">
+        <v>97.125867195242805</v>
+      </c>
+      <c r="F25" s="9">
+        <v>96.1347869177403</v>
+      </c>
+      <c r="G25" s="9">
+        <v>96.630327056491495</v>
+      </c>
+      <c r="H25" s="8">
+        <v>97.522299306243795</v>
+      </c>
+      <c r="I25" s="9">
+        <v>96.333002973240795</v>
+      </c>
+      <c r="J25" s="9">
+        <v>95.738354806739295</v>
+      </c>
+      <c r="K25" s="9">
+        <v>95.639246778989005</v>
+      </c>
+      <c r="L25" s="13">
+        <v>97.0267591674925</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0.20408163265306101</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0.10204081632653</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f>A28+1</f>
+        <v>1</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0</v>
+      </c>
+      <c r="D29" s="12">
+        <v>6.2555066079295099</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>0</v>
+      </c>
+      <c r="L29" s="8">
+        <v>8.8105726872246701E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" ref="A30:A37" si="2">A29+1</f>
+        <v>2</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8">
+        <v>9.68992248062015E-2</v>
+      </c>
+      <c r="D30" s="8">
+        <v>9.68992248062015E-2</v>
+      </c>
+      <c r="E30" s="12">
+        <v>9.68992248062015E-2</v>
+      </c>
+      <c r="F30" s="8">
+        <v>9.68992248062015E-2</v>
+      </c>
+      <c r="G30" s="8">
+        <v>0.290697674418604</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0</v>
+      </c>
+      <c r="I30" s="9">
+        <v>0</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
+      <c r="K30" s="8">
+        <v>9.68992248062015E-2</v>
+      </c>
+      <c r="L30" s="8">
+        <v>0.775193798449612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="12">
+        <v>22.574257425742498</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0.29702970297029702</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1.58415841584158</v>
+      </c>
+      <c r="I31" s="8">
+        <v>9.9009900990099001E-2</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+      <c r="K31" s="8">
+        <v>0.198019801980198</v>
+      </c>
+      <c r="L31" s="8">
+        <v>0.49504950495049499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.20366598778004</v>
+      </c>
+      <c r="G32" s="12">
+        <v>0.20366598778004</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="I32" s="9">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0.10183299389002</v>
+      </c>
+      <c r="L32" s="8">
+        <v>0.20366598778004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
+      <c r="B33" s="7">
+        <v>0.112107623318385</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.224215246636771</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.112107623318385</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0.112107623318385</v>
+      </c>
+      <c r="F33" s="8">
+        <v>4.9327354260089598</v>
+      </c>
+      <c r="G33" s="8">
+        <v>1.12107623318385</v>
+      </c>
+      <c r="H33" s="12">
+        <v>13.7892376681614</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0.56053811659192798</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.112107623318385</v>
+      </c>
+      <c r="K33" s="8">
+        <v>0.224215246636771</v>
+      </c>
+      <c r="L33" s="8">
+        <v>1.12107623318385</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0.73068893528183698</v>
+      </c>
+      <c r="C34" s="8">
+        <v>3.2359081419624198</v>
+      </c>
+      <c r="D34" s="8">
+        <v>0.83507306889352795</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1.7745302713987401</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.93945720250521902</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0.62630480167014602</v>
+      </c>
+      <c r="H34" s="8">
+        <v>0.93945720250521902</v>
+      </c>
+      <c r="I34" s="12">
+        <v>4.6972860125260896</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0.73068893528183698</v>
+      </c>
+      <c r="K34" s="8">
+        <v>1.25260960334029</v>
+      </c>
+      <c r="L34" s="8">
+        <v>2.0876826722338202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B35" s="7">
+        <v>100</v>
+      </c>
+      <c r="C35" s="9">
+        <v>100</v>
+      </c>
+      <c r="D35" s="9">
+        <v>100</v>
+      </c>
+      <c r="E35" s="9">
+        <v>100</v>
+      </c>
+      <c r="F35" s="9">
+        <v>100</v>
+      </c>
+      <c r="G35" s="9">
+        <v>100</v>
+      </c>
+      <c r="H35" s="9">
+        <v>100</v>
+      </c>
+      <c r="I35" s="9">
+        <v>100</v>
+      </c>
+      <c r="J35" s="12">
+        <v>100</v>
+      </c>
+      <c r="K35" s="9">
+        <v>100</v>
+      </c>
+      <c r="L35" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0.102669404517453</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0.102669404517453</v>
+      </c>
+      <c r="F36" s="8">
+        <v>1.84804928131416</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0</v>
+      </c>
+      <c r="I36" s="9">
+        <v>0</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
+      <c r="K36" s="12">
+        <v>1.2320328542094401</v>
+      </c>
+      <c r="L36" s="8">
+        <v>0.102669404517453</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0</v>
+      </c>
+      <c r="F37" s="8">
+        <v>9.9108027750247699E-2</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0</v>
+      </c>
+      <c r="I37" s="9">
+        <v>0</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0</v>
+      </c>
+      <c r="L37" s="12">
+        <v>9.9108027750247699E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7C8AE8-68EA-4CD1-89FD-4632DB72F050}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0.16</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.18</v>
+      </c>
+      <c r="D3" s="14">
+        <v>6.26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.68</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.59</v>
+      </c>
+      <c r="D5" s="14">
+        <v>22.57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.92</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="14">
+        <v>-0.02</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0.67</v>
+      </c>
+      <c r="D7" s="14">
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0.73</v>
+      </c>
+      <c r="D8" s="14">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.51</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="14">
+        <v>-1.8</v>
+      </c>
+      <c r="C11" s="14">
+        <v>-0.2</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>